<commit_message>
Excel Import, Multiple Documents upload
</commit_message>
<xml_diff>
--- a/public/files/import_from_excel_format.xlsx
+++ b/public/files/import_from_excel_format.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="93">
   <si>
     <t>NAME</t>
   </si>
@@ -214,62 +214,92 @@
     <t>Import10</t>
   </si>
   <si>
-    <t>import1@gmail.com1</t>
-  </si>
-  <si>
     <t>import1@gmail.com2</t>
   </si>
   <si>
     <t>import1@gmail.com3</t>
   </si>
   <si>
+    <t>import1@gmail.com5</t>
+  </si>
+  <si>
+    <t>import1@gmail.com6</t>
+  </si>
+  <si>
+    <t>import1@gmail.com7</t>
+  </si>
+  <si>
+    <t>import1@gmail.com8</t>
+  </si>
+  <si>
+    <t>import1@gmail.com9</t>
+  </si>
+  <si>
+    <t>import1@gmail.com10</t>
+  </si>
+  <si>
+    <t>PASSWORD</t>
+  </si>
+  <si>
+    <t>GENDER</t>
+  </si>
+  <si>
+    <t>HOURLY_RATE</t>
+  </si>
+  <si>
+    <t>ANNUAL_SALARY</t>
+  </si>
+  <si>
+    <t>START_DATE</t>
+  </si>
+  <si>
+    <t>USER_TYPE</t>
+  </si>
+  <si>
+    <t>client</t>
+  </si>
+  <si>
     <t>import1@gmail.com4</t>
   </si>
   <si>
-    <t>import1@gmail.com5</t>
-  </si>
-  <si>
-    <t>import1@gmail.com6</t>
-  </si>
-  <si>
-    <t>import1@gmail.com7</t>
-  </si>
-  <si>
-    <t>import1@gmail.com8</t>
-  </si>
-  <si>
-    <t>import1@gmail.com9</t>
-  </si>
-  <si>
-    <t>import1@gmail.com10</t>
-  </si>
-  <si>
-    <t>PASSWORD</t>
-  </si>
-  <si>
-    <t>GENDER</t>
-  </si>
-  <si>
-    <t>HOURLY_RATE</t>
-  </si>
-  <si>
-    <t>ANNUAL_SALARY</t>
-  </si>
-  <si>
-    <t>START_DATE</t>
-  </si>
-  <si>
-    <t>USER_TYPE</t>
-  </si>
-  <si>
-    <t>client</t>
+    <t>male12342</t>
+  </si>
+  <si>
+    <t>male12343</t>
+  </si>
+  <si>
+    <t>male12344</t>
+  </si>
+  <si>
+    <t>male12345</t>
+  </si>
+  <si>
+    <t>male12346</t>
+  </si>
+  <si>
+    <t>male12347</t>
+  </si>
+  <si>
+    <t>male12348</t>
+  </si>
+  <si>
+    <t>male12349</t>
+  </si>
+  <si>
+    <t>male12350</t>
+  </si>
+  <si>
+    <t>male12351</t>
+  </si>
+  <si>
+    <t>asdfasdf@fasdf.om</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -286,16 +316,34 @@
       <color theme="10"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -303,15 +351,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -617,18 +684,18 @@
   <dimension ref="A1:W11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
     <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="24.7109375" bestFit="1" customWidth="1"/>
@@ -637,41 +704,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="I1" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="6" t="s">
         <v>79</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -686,14 +753,14 @@
       <c r="W1" s="1"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>56</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>82</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -717,18 +784,18 @@
         <v>10</v>
       </c>
       <c r="L2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>83</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -755,18 +822,18 @@
         <v>15</v>
       </c>
       <c r="L3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="D4" t="s">
         <v>16</v>
@@ -793,18 +860,18 @@
         <v>21</v>
       </c>
       <c r="L4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>85</v>
       </c>
       <c r="D5" t="s">
         <v>6</v>
@@ -831,18 +898,18 @@
         <v>26</v>
       </c>
       <c r="L5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>60</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>86</v>
       </c>
       <c r="D6" t="s">
         <v>6</v>
@@ -869,18 +936,18 @@
         <v>31</v>
       </c>
       <c r="L6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>61</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="D7" t="s">
         <v>6</v>
@@ -907,18 +974,18 @@
         <v>36</v>
       </c>
       <c r="L7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>62</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>88</v>
       </c>
       <c r="D8" t="s">
         <v>6</v>
@@ -945,18 +1012,18 @@
         <v>41</v>
       </c>
       <c r="L8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>63</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>89</v>
       </c>
       <c r="D9" t="s">
         <v>16</v>
@@ -983,18 +1050,18 @@
         <v>46</v>
       </c>
       <c r="L9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="3" t="s">
         <v>64</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>90</v>
       </c>
       <c r="D10" t="s">
         <v>6</v>
@@ -1021,18 +1088,18 @@
         <v>51</v>
       </c>
       <c r="L10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="3" t="s">
         <v>65</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>91</v>
       </c>
       <c r="D11" t="s">
         <v>6</v>
@@ -1056,15 +1123,15 @@
         <v>55</v>
       </c>
       <c r="L11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3:B11" r:id="rId2" display="import1@gmail.com1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>